<commit_message>
10 correções de vários erros;
2) adicionando INTERVALOR p/ o projeto;
</commit_message>
<xml_diff>
--- a/CoParticipacaoWebService/src/test/resources/cargill/input/CARGILL.NAO-LOCALIZADO.201807.003.xlsx
+++ b/CoParticipacaoWebService/src/test/resources/cargill/input/CARGILL.NAO-LOCALIZADO.201807.003.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="00192" sheetId="1" state="visible" r:id="rId2"/>
@@ -168,7 +168,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -181,15 +181,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -272,8 +268,8 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -324,10 +320,10 @@
         <v>9</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>17262</v>
+        <v>17261</v>
       </c>
       <c r="G2" s="4" t="n">
-        <v>43357</v>
+        <v>41653</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -347,10 +343,10 @@
         <v>9</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>17263</v>
+        <v>17261</v>
       </c>
       <c r="G3" s="4" t="n">
-        <v>43357</v>
+        <v>41653</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -373,7 +369,7 @@
         <v>17261</v>
       </c>
       <c r="G4" s="4" t="n">
-        <v>43357</v>
+        <v>41653</v>
       </c>
     </row>
   </sheetData>
@@ -394,8 +390,8 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -436,8 +432,8 @@
       <c r="B2" s="2" t="n">
         <v>400224375</v>
       </c>
-      <c r="C2" s="5" t="n">
-        <v>80474075036</v>
+      <c r="C2" s="3" t="n">
+        <v>64839810079</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>13</v>
@@ -446,10 +442,10 @@
         <v>9</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>17263</v>
+        <v>17260</v>
       </c>
       <c r="G2" s="4" t="n">
-        <v>43337</v>
+        <v>38132</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -459,8 +455,8 @@
       <c r="B3" s="2" t="n">
         <v>400311895</v>
       </c>
-      <c r="C3" s="5" t="n">
-        <v>38849177062</v>
+      <c r="C3" s="3" t="n">
+        <v>34459123002</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>14</v>
@@ -469,10 +465,10 @@
         <v>9</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>17261</v>
+        <v>17260</v>
       </c>
       <c r="G3" s="4" t="n">
-        <v>43337</v>
+        <v>38132</v>
       </c>
     </row>
   </sheetData>
@@ -494,7 +490,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>